<commit_message>
new inputs and outputs
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natomanzolli/Documents/GitHub/Drive-Tech/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97968751-466B-B542-9FF4-5C454E78AED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6912F6-A3EB-1D4C-981F-EA32444D30CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="3640" windowWidth="27840" windowHeight="16740" activeTab="1" xr2:uid="{B5AC5AED-6860-8F4C-AD59-578B1B31F775}"/>
+    <workbookView xWindow="2400" yWindow="2880" windowWidth="27840" windowHeight="16740" xr2:uid="{B5AC5AED-6860-8F4C-AD59-578B1B31F775}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
   <si>
     <t>Buses</t>
   </si>
@@ -70,6 +70,57 @@
   </si>
   <si>
     <t>Velocity (average)</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>BYD</t>
+  </si>
+  <si>
+    <t>Mercedez</t>
+  </si>
+  <si>
+    <t>Man</t>
+  </si>
+  <si>
+    <t>Volvo</t>
+  </si>
+  <si>
+    <t>Karsan</t>
+  </si>
+  <si>
+    <t>Bus Brand</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>SOH</t>
+  </si>
+  <si>
+    <t>Bus ID</t>
+  </si>
+  <si>
+    <t>Charger ID</t>
+  </si>
+  <si>
+    <t>Siemens</t>
+  </si>
+  <si>
+    <t>ABB</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Unidirectional</t>
+  </si>
+  <si>
+    <t>Line ID</t>
+  </si>
+  <si>
+    <t>Round-trips</t>
   </si>
 </sst>
 </file>
@@ -79,10 +130,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -445,858 +502,1400 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4266C8-C06D-EC47-84E6-8FB83C00A693}">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="10" max="12" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="Q1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>200</v>
       </c>
-      <c r="B2">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>98</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="C2">
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2">
         <f>Calculation!C2*Calculation!D2/Calculation!A2</f>
         <v>2.7</v>
       </c>
-      <c r="D2">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>10</v>
+      </c>
+      <c r="M2">
         <f>Calculation!E2*Calculation!$A$2*24</f>
         <v>24</v>
       </c>
-      <c r="E2">
+      <c r="N2">
         <f>Calculation!F2*24*Calculation!$A$2</f>
         <v>72</v>
       </c>
-      <c r="F2">
+      <c r="O2">
+        <v>20</v>
+      </c>
+      <c r="P2">
         <v>9.6196376021798355E-2</v>
       </c>
-      <c r="G2">
+      <c r="Q2">
         <v>50</v>
       </c>
-      <c r="H2">
+      <c r="R2">
         <f>1.7125*1</f>
         <v>1.7124999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>200</v>
       </c>
-      <c r="B3">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>99</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D3">
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>11</v>
+      </c>
+      <c r="M3">
         <f>Calculation!E3*Calculation!$A$2*24</f>
         <v>25</v>
       </c>
-      <c r="E3">
+      <c r="N3">
         <f>Calculation!F3*24*Calculation!$A$2</f>
         <v>76</v>
       </c>
-      <c r="F3">
+      <c r="O3">
+        <v>25</v>
+      </c>
+      <c r="P3">
         <v>9.6196376021798355E-2</v>
       </c>
-      <c r="G3">
+      <c r="Q3">
         <v>100</v>
       </c>
-      <c r="H3">
+      <c r="R3">
         <f>1.7125*2</f>
         <v>3.4249999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>200</v>
       </c>
-      <c r="B4">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D4">
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>20</v>
+      </c>
+      <c r="M4">
         <f>Calculation!E4*Calculation!$A$2*24</f>
         <v>26</v>
       </c>
-      <c r="E4">
+      <c r="N4">
         <f>Calculation!F4*24*Calculation!$A$2</f>
         <v>74</v>
       </c>
-      <c r="F4">
+      <c r="O4">
+        <v>30</v>
+      </c>
+      <c r="P4">
         <v>9.6196376021798355E-2</v>
       </c>
-      <c r="G4">
+      <c r="Q4">
         <v>150</v>
       </c>
-      <c r="H4">
+      <c r="R4">
         <f>1.7125*3</f>
         <v>5.1374999999999993</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>200</v>
       </c>
-      <c r="B5">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D5">
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>8</v>
+      </c>
+      <c r="M5">
         <f>Calculation!E5*Calculation!$A$2*24</f>
         <v>27</v>
       </c>
-      <c r="E5">
+      <c r="N5">
         <f>Calculation!F5*24*Calculation!$A$2</f>
         <v>79</v>
       </c>
-      <c r="F5">
+      <c r="O5">
+        <v>40</v>
+      </c>
+      <c r="P5">
         <v>9.6196376021798355E-2</v>
       </c>
-      <c r="G5">
+      <c r="Q5">
         <v>200</v>
       </c>
-      <c r="H5">
+      <c r="R5">
         <f>1.7125*4</f>
         <v>6.85</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>200</v>
       </c>
-      <c r="B6">
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+      <c r="G6">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D6">
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>7</v>
+      </c>
+      <c r="M6">
         <f>Calculation!E6*Calculation!$A$2*24</f>
         <v>28</v>
       </c>
-      <c r="E6">
+      <c r="N6">
         <f>Calculation!F6*24*Calculation!$A$2</f>
         <v>81</v>
       </c>
-      <c r="F6">
+      <c r="O6">
+        <v>35</v>
+      </c>
+      <c r="P6">
         <v>8.8765994550408719E-2</v>
       </c>
-      <c r="G6">
+      <c r="Q6">
         <v>250</v>
       </c>
-      <c r="H6">
+      <c r="R6">
         <f>1.7125*5</f>
         <v>8.5625</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>200</v>
       </c>
-      <c r="B7">
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D7">
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>13</v>
+      </c>
+      <c r="M7">
         <f>Calculation!E7*Calculation!$A$2*24</f>
         <v>29</v>
       </c>
-      <c r="E7">
+      <c r="N7">
         <f>Calculation!F7*24*Calculation!$A$2</f>
         <v>78</v>
       </c>
-      <c r="F7">
+      <c r="O7">
+        <v>20</v>
+      </c>
+      <c r="P7">
         <v>8.8765994550408719E-2</v>
       </c>
-      <c r="G7">
+      <c r="Q7">
         <v>300</v>
       </c>
-      <c r="H7">
+      <c r="R7">
         <f>1.7125*6</f>
         <v>10.274999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>200</v>
       </c>
-      <c r="B8">
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D8">
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8">
+        <v>7</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
         <f>Calculation!E8*Calculation!$A$2*24</f>
         <v>30</v>
       </c>
-      <c r="E8">
+      <c r="N8">
         <f>Calculation!F8*24*Calculation!$A$2</f>
         <v>80</v>
       </c>
-      <c r="F8">
+      <c r="O8">
+        <v>35</v>
+      </c>
+      <c r="P8">
         <v>8.8765994550408719E-2</v>
       </c>
-      <c r="G8">
+      <c r="Q8">
         <v>450</v>
       </c>
-      <c r="H8">
+      <c r="R8">
         <f>1.7125*7</f>
         <v>11.987499999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>200</v>
       </c>
-      <c r="B9">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D9">
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>8</v>
+      </c>
+      <c r="L9">
+        <v>9</v>
+      </c>
+      <c r="M9">
         <f>Calculation!E9*Calculation!$A$2*24</f>
         <v>31</v>
       </c>
-      <c r="E9">
+      <c r="N9">
         <f>Calculation!F9*24*Calculation!$A$2</f>
         <v>78</v>
       </c>
-      <c r="F9">
+      <c r="O9">
+        <v>35</v>
+      </c>
+      <c r="P9">
         <v>8.8765994550408719E-2</v>
       </c>
-      <c r="G9">
+      <c r="Q9">
         <v>500</v>
       </c>
-      <c r="H9">
+      <c r="R9">
         <f>1.7125*8</f>
         <v>13.7</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>200</v>
       </c>
-      <c r="B10">
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10">
+        <v>99</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D10">
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="L10">
+        <v>15</v>
+      </c>
+      <c r="M10">
         <f>Calculation!E10*Calculation!$A$2*24</f>
         <v>32</v>
       </c>
-      <c r="E10">
+      <c r="N10">
         <f>Calculation!F10*24*Calculation!$A$2</f>
         <v>84</v>
       </c>
-      <c r="F10">
+      <c r="O10">
+        <v>25</v>
+      </c>
+      <c r="P10">
         <v>8.4496621253405985E-2</v>
       </c>
-      <c r="G10">
+      <c r="Q10">
         <v>550</v>
       </c>
-      <c r="H10">
+      <c r="R10">
         <f>1.7125*9</f>
         <v>15.4125</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
         <v>200</v>
       </c>
-      <c r="B11">
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+      <c r="E11">
+        <v>97</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+      <c r="G11">
         <f>Calculation!$B$2/Calculation!$A$2</f>
         <v>25</v>
       </c>
-      <c r="D11">
+      <c r="H11" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>10</v>
+      </c>
+      <c r="L11">
+        <v>11</v>
+      </c>
+      <c r="M11">
         <f>Calculation!E11*Calculation!$A$2*24</f>
         <v>24</v>
       </c>
-      <c r="E11">
+      <c r="N11">
         <f>Calculation!F11*24*Calculation!$A$2</f>
         <v>72</v>
       </c>
-      <c r="F11">
+      <c r="O11">
+        <v>32</v>
+      </c>
+      <c r="P11">
         <v>8.4496621253405985E-2</v>
       </c>
-      <c r="G11">
+      <c r="Q11">
         <v>600</v>
       </c>
-      <c r="H11">
+      <c r="R11">
         <f>1.7125*10</f>
         <v>17.125</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
         <v>200</v>
       </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
       <c r="D12">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>95</v>
+      </c>
+      <c r="K12">
+        <v>11</v>
+      </c>
+      <c r="L12">
+        <v>16</v>
+      </c>
+      <c r="M12">
         <f>Calculation!E12*Calculation!$A$2*24</f>
         <v>25</v>
       </c>
-      <c r="E12">
+      <c r="N12">
         <f>Calculation!F12*24*Calculation!$A$2</f>
         <v>76</v>
       </c>
-      <c r="F12">
+      <c r="O12">
+        <v>28</v>
+      </c>
+      <c r="P12">
         <v>8.4496621253405985E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
         <v>200</v>
       </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
       <c r="D13">
+        <v>12</v>
+      </c>
+      <c r="E13">
+        <v>99</v>
+      </c>
+      <c r="K13">
+        <v>12</v>
+      </c>
+      <c r="L13">
+        <v>19</v>
+      </c>
+      <c r="M13">
         <f>Calculation!E13*Calculation!$A$2*24</f>
         <v>26</v>
       </c>
-      <c r="E13">
+      <c r="N13">
         <f>Calculation!F13*24*Calculation!$A$2</f>
         <v>74</v>
       </c>
-      <c r="F13">
+      <c r="O13">
+        <v>15</v>
+      </c>
+      <c r="P13">
         <v>8.4496621253405985E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
         <v>200</v>
       </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
       <c r="D14">
+        <v>18</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="K14">
+        <v>13</v>
+      </c>
+      <c r="L14">
+        <v>21</v>
+      </c>
+      <c r="M14">
         <f>Calculation!E14*Calculation!$A$2*24</f>
         <v>27</v>
       </c>
-      <c r="E14">
+      <c r="N14">
         <f>Calculation!F14*24*Calculation!$A$2</f>
         <v>79</v>
       </c>
-      <c r="F14">
+      <c r="O14">
+        <v>12</v>
+      </c>
+      <c r="P14">
         <v>8.2280217983651233E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
         <v>200</v>
       </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
       <c r="D15">
+        <v>18</v>
+      </c>
+      <c r="E15">
+        <v>99</v>
+      </c>
+      <c r="K15">
+        <v>14</v>
+      </c>
+      <c r="L15">
+        <v>10</v>
+      </c>
+      <c r="M15">
         <f>Calculation!E15*Calculation!$A$2*24</f>
         <v>28</v>
       </c>
-      <c r="E15">
+      <c r="N15">
         <f>Calculation!F15*24*Calculation!$A$2</f>
         <v>81</v>
       </c>
-      <c r="F15">
+      <c r="O15">
+        <v>40</v>
+      </c>
+      <c r="P15">
         <v>8.2280217983651233E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>200</v>
       </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
       <c r="D16">
+        <v>18</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="K16">
+        <v>15</v>
+      </c>
+      <c r="L16">
+        <v>25</v>
+      </c>
+      <c r="M16">
         <f>Calculation!E16*Calculation!$A$2*24</f>
         <v>29</v>
       </c>
-      <c r="E16">
+      <c r="N16">
         <f>Calculation!F16*24*Calculation!$A$2</f>
         <v>78</v>
       </c>
-      <c r="F16">
+      <c r="O16">
+        <v>12</v>
+      </c>
+      <c r="P16">
         <v>8.2280217983651233E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
         <v>200</v>
       </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
       <c r="D17">
+        <v>12</v>
+      </c>
+      <c r="E17">
+        <v>96</v>
+      </c>
+      <c r="K17">
+        <v>16</v>
+      </c>
+      <c r="L17">
+        <v>11</v>
+      </c>
+      <c r="M17">
         <f>Calculation!E17*Calculation!$A$2*24</f>
         <v>30</v>
       </c>
-      <c r="E17">
+      <c r="N17">
         <f>Calculation!F17*24*Calculation!$A$2</f>
         <v>80</v>
       </c>
-      <c r="F17">
+      <c r="O17">
+        <v>30</v>
+      </c>
+      <c r="P17">
         <v>8.2280217983651233E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>200</v>
       </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
       <c r="D18">
+        <v>12</v>
+      </c>
+      <c r="E18">
+        <v>99</v>
+      </c>
+      <c r="K18">
+        <v>17</v>
+      </c>
+      <c r="L18">
+        <v>7</v>
+      </c>
+      <c r="M18">
         <f>Calculation!E18*Calculation!$A$2*24</f>
         <v>31</v>
       </c>
-      <c r="E18">
+      <c r="N18">
         <f>Calculation!F18*24*Calculation!$A$2</f>
         <v>78</v>
       </c>
-      <c r="F18">
+      <c r="O18">
+        <v>31</v>
+      </c>
+      <c r="P18">
         <v>8.0808038147138953E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>200</v>
       </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
       <c r="D19">
+        <v>12</v>
+      </c>
+      <c r="E19">
+        <v>95</v>
+      </c>
+      <c r="K19">
+        <v>18</v>
+      </c>
+      <c r="L19">
+        <v>18</v>
+      </c>
+      <c r="M19">
         <f>Calculation!E19*Calculation!$A$2*24</f>
         <v>32</v>
       </c>
-      <c r="E19">
+      <c r="N19">
         <f>Calculation!F19*24*Calculation!$A$2</f>
         <v>84</v>
       </c>
-      <c r="F19">
+      <c r="O19">
+        <v>12</v>
+      </c>
+      <c r="P19">
         <v>8.0808038147138953E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
         <v>200</v>
       </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
       <c r="D20">
+        <v>10</v>
+      </c>
+      <c r="E20">
+        <v>97</v>
+      </c>
+      <c r="K20">
+        <v>19</v>
+      </c>
+      <c r="L20">
+        <v>17</v>
+      </c>
+      <c r="M20">
         <f>Calculation!E20*Calculation!$A$2*24</f>
         <v>20</v>
       </c>
-      <c r="E20">
+      <c r="N20">
         <f>Calculation!F20*24*Calculation!$A$2</f>
         <v>72</v>
       </c>
-      <c r="F20">
+      <c r="O20">
+        <v>15</v>
+      </c>
+      <c r="P20">
         <v>8.0808038147138953E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
         <v>200</v>
       </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
       <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>99</v>
+      </c>
+      <c r="K21">
+        <v>20</v>
+      </c>
+      <c r="L21">
+        <v>22</v>
+      </c>
+      <c r="M21">
         <f>Calculation!E21*Calculation!$A$2*24</f>
         <v>41</v>
       </c>
-      <c r="E21">
+      <c r="N21">
         <f>Calculation!F21*24*Calculation!$A$2</f>
         <v>92</v>
       </c>
-      <c r="F21">
+      <c r="O21">
+        <v>12</v>
+      </c>
+      <c r="P21">
         <v>8.0808038147138953E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F22">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P22">
         <v>8.3833242506811984E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F23">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P23">
         <v>8.3833242506811984E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F24">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P24">
         <v>8.3833242506811984E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P25">
         <v>8.3833242506811984E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F26">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P26">
         <v>9.2526267029972756E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F27">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P27">
         <v>9.2526267029972756E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F28">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P28">
         <v>9.2526267029972756E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F29">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P29">
         <v>9.2526267029972756E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F30">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P30">
         <v>0.102791280653951</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F31">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P31">
         <v>0.102791280653951</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F32">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P32">
         <v>0.102791280653951</v>
       </c>
     </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F33">
+    <row r="33" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P33">
         <v>0.102791280653951</v>
       </c>
     </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F34">
+    <row r="34" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P34">
         <v>0.10571716621253401</v>
       </c>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F35">
+    <row r="35" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P35">
         <v>0.10571716621253401</v>
       </c>
     </row>
-    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F36">
+    <row r="36" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P36">
         <v>0.10571716621253401</v>
       </c>
     </row>
-    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F37">
+    <row r="37" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P37">
         <v>0.10571716621253401</v>
       </c>
     </row>
-    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F38">
+    <row r="38" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P38">
         <v>9.5729809264305174E-2</v>
       </c>
     </row>
-    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F39">
+    <row r="39" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P39">
         <v>9.5729809264305174E-2</v>
       </c>
     </row>
-    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F40">
+    <row r="40" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P40">
         <v>9.5729809264305174E-2</v>
       </c>
     </row>
-    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F41">
+    <row r="41" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P41">
         <v>9.5729809264305174E-2</v>
       </c>
     </row>
-    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F42">
+    <row r="42" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P42">
         <v>8.299574931880109E-2</v>
       </c>
     </row>
-    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F43">
+    <row r="43" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P43">
         <v>8.299574931880109E-2</v>
       </c>
     </row>
-    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F44">
+    <row r="44" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P44">
         <v>8.299574931880109E-2</v>
       </c>
     </row>
-    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F45">
+    <row r="45" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P45">
         <v>8.299574931880109E-2</v>
       </c>
     </row>
-    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F46">
+    <row r="46" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P46">
         <v>7.7228310626703003E-2</v>
       </c>
     </row>
-    <row r="47" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F47">
+    <row r="47" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P47">
         <v>7.7228310626703003E-2</v>
       </c>
     </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F48">
+    <row r="48" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P48">
         <v>7.7228310626703003E-2</v>
       </c>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F49">
+    <row r="49" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P49">
         <v>7.7228310626703003E-2</v>
       </c>
     </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F50">
+    <row r="50" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P50">
         <v>7.4376866485013626E-2</v>
       </c>
     </row>
-    <row r="51" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F51">
+    <row r="51" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P51">
         <v>7.4376866485013626E-2</v>
       </c>
     </row>
-    <row r="52" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F52">
+    <row r="52" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P52">
         <v>7.4376866485013626E-2</v>
       </c>
     </row>
-    <row r="53" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F53">
+    <row r="53" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P53">
         <v>7.4376866485013626E-2</v>
       </c>
     </row>
-    <row r="54" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F54">
+    <row r="54" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P54">
         <v>7.1927956403269766E-2</v>
       </c>
     </row>
-    <row r="55" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F55">
+    <row r="55" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P55">
         <v>7.1927956403269766E-2</v>
       </c>
     </row>
-    <row r="56" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F56">
+    <row r="56" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P56">
         <v>7.1927956403269766E-2</v>
       </c>
     </row>
-    <row r="57" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F57">
+    <row r="57" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P57">
         <v>7.1927956403269766E-2</v>
       </c>
     </row>
-    <row r="58" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F58">
+    <row r="58" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P58">
         <v>6.8611035422343314E-2</v>
       </c>
     </row>
-    <row r="59" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F59">
+    <row r="59" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P59">
         <v>6.8611035422343314E-2</v>
       </c>
     </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F60">
+    <row r="60" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P60">
         <v>6.8611035422343314E-2</v>
       </c>
     </row>
-    <row r="61" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F61">
+    <row r="61" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P61">
         <v>6.8611035422343314E-2</v>
       </c>
     </row>
-    <row r="62" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F62">
+    <row r="62" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P62">
         <v>6.7398910081743882E-2</v>
       </c>
     </row>
-    <row r="63" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F63">
+    <row r="63" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P63">
         <v>6.7398910081743882E-2</v>
       </c>
     </row>
-    <row r="64" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F64">
+    <row r="64" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P64">
         <v>6.7398910081743882E-2</v>
       </c>
     </row>
-    <row r="65" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F65">
+    <row r="65" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P65">
         <v>6.7398910081743882E-2</v>
       </c>
     </row>
-    <row r="66" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F66">
+    <row r="66" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P66">
         <v>7.1017929155313353E-2</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F67">
+    <row r="67" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P67">
         <v>7.1017929155313353E-2</v>
       </c>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F68">
+    <row r="68" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P68">
         <v>7.1017929155313353E-2</v>
       </c>
     </row>
-    <row r="69" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F69">
+    <row r="69" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P69">
         <v>7.1017929155313353E-2</v>
       </c>
     </row>
-    <row r="70" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F70">
+    <row r="70" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P70">
         <v>8.1150626702997275E-2</v>
       </c>
     </row>
-    <row r="71" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F71">
+    <row r="71" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P71">
         <v>8.1150626702997275E-2</v>
       </c>
     </row>
-    <row r="72" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F72">
+    <row r="72" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P72">
         <v>8.1150626702997275E-2</v>
       </c>
     </row>
-    <row r="73" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F73">
+    <row r="73" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P73">
         <v>8.1150626702997275E-2</v>
       </c>
     </row>
-    <row r="74" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F74">
+    <row r="74" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P74">
         <v>9.4181198910081754E-2</v>
       </c>
     </row>
-    <row r="75" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F75">
+    <row r="75" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P75">
         <v>9.4181198910081754E-2</v>
       </c>
     </row>
-    <row r="76" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F76">
+    <row r="76" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P76">
         <v>9.4181198910081754E-2</v>
       </c>
     </row>
-    <row r="77" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F77">
+    <row r="77" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P77">
         <v>9.4181198910081754E-2</v>
       </c>
     </row>
-    <row r="78" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F78">
+    <row r="78" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P78">
         <v>0.11045356948228879</v>
       </c>
     </row>
-    <row r="79" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F79">
+    <row r="79" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P79">
         <v>0.11045356948228879</v>
       </c>
     </row>
-    <row r="80" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F80">
+    <row r="80" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P80">
         <v>0.11045356948228879</v>
       </c>
     </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F81">
+    <row r="81" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P81">
         <v>0.11045356948228879</v>
       </c>
     </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F82">
+    <row r="82" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P82">
         <v>0.1221265940054496</v>
       </c>
     </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F83">
+    <row r="83" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P83">
         <v>0.1221265940054496</v>
       </c>
     </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F84">
+    <row r="84" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P84">
         <v>0.1221265940054496</v>
       </c>
     </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F85">
+    <row r="85" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P85">
         <v>0.1221265940054496</v>
       </c>
     </row>
-    <row r="86" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F86">
+    <row r="86" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P86">
         <v>0.12058182561307899</v>
       </c>
     </row>
-    <row r="87" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F87">
+    <row r="87" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P87">
         <v>0.12058182561307899</v>
       </c>
     </row>
-    <row r="88" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F88">
+    <row r="88" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P88">
         <v>0.12058182561307899</v>
       </c>
     </row>
-    <row r="89" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F89">
+    <row r="89" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P89">
         <v>0.12058182561307899</v>
       </c>
     </row>
-    <row r="90" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F90">
+    <row r="90" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P90">
         <v>0.1114515803814714</v>
       </c>
     </row>
-    <row r="91" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F91">
+    <row r="91" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P91">
         <v>0.1114515803814714</v>
       </c>
     </row>
-    <row r="92" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F92">
+    <row r="92" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P92">
         <v>0.1114515803814714</v>
       </c>
     </row>
-    <row r="93" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F93">
+    <row r="93" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P93">
         <v>0.1114515803814714</v>
       </c>
     </row>
-    <row r="94" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F94">
+    <row r="94" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P94">
         <v>0.1015224043715847</v>
       </c>
     </row>
-    <row r="95" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F95">
+    <row r="95" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P95">
         <v>0.1015224043715847</v>
       </c>
     </row>
-    <row r="96" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F96">
+    <row r="96" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P96">
         <v>0.1015224043715847</v>
       </c>
     </row>
-    <row r="97" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F97">
+    <row r="97" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P97">
         <v>0.1015224043715847</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1305,8 +1904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0BDDA4-3ED4-5A46-AA6F-5591465BF29F}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>